<commit_message>
Site updated: 2023-01-19 18:45:09
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE2524E-847A-49D3-9C4F-429E8D638C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAB4E07-DF45-48A2-A3A6-64411CDFBFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -619,6 +616,15 @@
     <xf numFmtId="176" fontId="3" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="5" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -634,34 +640,25 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="5" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -682,19 +679,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -963,7 +947,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -977,22 +961,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1027,7 +1011,9 @@
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="6">
+        <v>44945</v>
+      </c>
       <c r="D4" s="7"/>
       <c r="E4" s="5"/>
       <c r="F4" s="8"/>
@@ -1039,7 +1025,9 @@
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6">
+        <v>44944</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="5"/>
       <c r="F5" s="8"/>
@@ -1051,7 +1039,9 @@
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6">
+        <v>44944</v>
+      </c>
       <c r="D6" s="7"/>
       <c r="E6" s="5"/>
       <c r="F6" s="8"/>
@@ -1063,20 +1053,22 @@
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6">
+        <v>44944</v>
+      </c>
       <c r="D7" s="7"/>
       <c r="E7" s="5"/>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="13"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1163,11 +1155,11 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="23"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="7"/>
       <c r="E16" s="5"/>
       <c r="F16" s="8"/>
@@ -1245,11 +1237,11 @@
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="16"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="23"/>
       <c r="D23" s="7"/>
       <c r="E23" s="5"/>
       <c r="F23" s="8"/>
@@ -1322,9 +1314,9 @@
         <v>24</v>
       </c>
       <c r="C29" s="6"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="13"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="16"/>
     </row>
     <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
@@ -1366,12 +1358,12 @@
       <c r="E33" s="5"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+    <row r="34" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="11"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="14"/>
       <c r="D34" s="7"/>
       <c r="E34" s="5"/>
       <c r="F34" s="8"/>
@@ -1408,9 +1400,9 @@
         <v>52</v>
       </c>
       <c r="C37" s="6"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="13"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="16"/>
     </row>
     <row r="38" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
@@ -1440,11 +1432,11 @@
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="6"/>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E40" s="10"/>
-      <c r="F40" s="11"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>

</xml_diff>

<commit_message>
Site updated: 2023-01-20 09:32:44
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAB4E07-DF45-48A2-A3A6-64411CDFBFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76F7C1D-87F7-427D-9D07-A6DF48295C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -947,7 +947,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1026,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="6">
-        <v>44944</v>
+        <v>44946</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="5"/>

</xml_diff>

<commit_message>
Site updated: 2023-01-21 11:30:47
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76F7C1D-87F7-427D-9D07-A6DF48295C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3284E982-D5D2-4977-81C9-99EE33EC5F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -947,7 +947,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1040,7 +1040,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="6">
-        <v>44944</v>
+        <v>44947</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="5"/>

</xml_diff>

<commit_message>
Site updated: 2023-01-22 11:46:15
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3284E982-D5D2-4977-81C9-99EE33EC5F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B20CE19-F203-483F-9756-DC3B172608A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -947,7 +947,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1054,7 +1054,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="6">
-        <v>44944</v>
+        <v>44948</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="5"/>

</xml_diff>

<commit_message>
Site updated: 2023-01-23 11:59:45
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B20CE19-F203-483F-9756-DC3B172608A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A31B5B-46FA-49FF-89A6-9D6A379079B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -947,7 +947,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1077,9 @@
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <v>44949</v>
+      </c>
       <c r="D9" s="7"/>
       <c r="E9" s="5"/>
       <c r="F9" s="8"/>
@@ -1089,7 +1091,9 @@
       <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="6">
+        <v>44949</v>
+      </c>
       <c r="D10" s="7"/>
       <c r="E10" s="5"/>
       <c r="F10" s="8"/>
@@ -1101,7 +1105,9 @@
       <c r="B11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6">
+        <v>44949</v>
+      </c>
       <c r="D11" s="7"/>
       <c r="E11" s="5"/>
       <c r="F11" s="8"/>
@@ -1113,7 +1119,9 @@
       <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="6">
+        <v>44949</v>
+      </c>
       <c r="D12" s="7"/>
       <c r="E12" s="5"/>
       <c r="F12" s="8"/>
@@ -1125,7 +1133,9 @@
       <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="6">
+        <v>44949</v>
+      </c>
       <c r="D13" s="7"/>
       <c r="E13" s="5"/>
       <c r="F13" s="8"/>
@@ -1137,7 +1147,9 @@
       <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="6">
+        <v>44949</v>
+      </c>
       <c r="D14" s="7"/>
       <c r="E14" s="5"/>
       <c r="F14" s="8"/>
@@ -1149,7 +1161,9 @@
       <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="6"/>
+      <c r="C15" s="6">
+        <v>44949</v>
+      </c>
       <c r="D15" s="7"/>
       <c r="E15" s="5"/>
       <c r="F15" s="8"/>

</xml_diff>

<commit_message>
Site updated: 2023-01-25 20:09:02
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A31B5B-46FA-49FF-89A6-9D6A379079B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F421DFBA-4D72-41BF-96DA-D4376C29D2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -947,7 +947,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1092,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="6">
-        <v>44949</v>
+        <v>44950</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="5"/>
@@ -1106,7 +1106,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="6">
-        <v>44949</v>
+        <v>44951</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="5"/>

</xml_diff>

<commit_message>
Site updated: 2023-01-26 19:05:54
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F421DFBA-4D72-41BF-96DA-D4376C29D2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388002F1-9DD4-4316-81E6-067A59DAA886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -947,7 +947,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1120,7 +1120,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="6">
-        <v>44949</v>
+        <v>44952</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="5"/>

</xml_diff>

<commit_message>
Site updated: 2023-01-27 13:05:05
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388002F1-9DD4-4316-81E6-067A59DAA886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B435005D-76DA-4020-A683-6CAD5649552D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -947,7 +947,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1134,7 +1134,7 @@
         <v>24</v>
       </c>
       <c r="C13" s="6">
-        <v>44949</v>
+        <v>44953</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="5"/>

</xml_diff>

<commit_message>
Site updated: 2023-01-28 12:02:28
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B435005D-76DA-4020-A683-6CAD5649552D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F408F89D-BE8A-4E7A-ACF6-8CF841104D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -947,7 +947,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1148,7 +1148,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="6">
-        <v>44949</v>
+        <v>44954</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="5"/>

</xml_diff>

<commit_message>
Site updated: 2023-01-29 13:31:20
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F408F89D-BE8A-4E7A-ACF6-8CF841104D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F6F881-0D58-4D06-B72F-EFCD1E1F3F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -947,7 +947,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1162,7 +1162,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="6">
-        <v>44949</v>
+        <v>44955</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="5"/>

</xml_diff>

<commit_message>
Site updated: 2023-01-30 11:18:19
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F6F881-0D58-4D06-B72F-EFCD1E1F3F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B138CA69-12E1-481D-A508-DCA02F4D9F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
   <si>
     <t>数组</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -947,7 +947,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1066,9 +1066,11 @@
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="22"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="16"/>
+      <c r="D8" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1080,9 +1082,13 @@
       <c r="C9" s="6">
         <v>44949</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="8"/>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1094,9 +1100,13 @@
       <c r="C10" s="6">
         <v>44950</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="8"/>
+      <c r="D10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -1108,9 +1118,13 @@
       <c r="C11" s="6">
         <v>44951</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="8"/>
+      <c r="D11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1122,9 +1136,13 @@
       <c r="C12" s="6">
         <v>44952</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="8"/>
+      <c r="D12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -1136,9 +1154,13 @@
       <c r="C13" s="6">
         <v>44953</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="8"/>
+      <c r="D13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -1150,9 +1172,13 @@
       <c r="C14" s="6">
         <v>44954</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="8"/>
+      <c r="D14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -1164,197 +1190,203 @@
       <c r="C15" s="6">
         <v>44955</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="8"/>
+      <c r="D15" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="23"/>
     </row>
     <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="8"/>
+      <c r="A16" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="8"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="8"/>
+      <c r="D18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="8"/>
+      <c r="D19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="8"/>
+      <c r="D20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="8"/>
+      <c r="D21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="8"/>
+      <c r="D22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>42</v>
-      </c>
+      <c r="A23" s="20"/>
       <c r="B23" s="21"/>
       <c r="C23" s="23"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="8"/>
+      <c r="D23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
+      <c r="D24" s="4"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="8"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="7"/>
+      <c r="D25" s="4"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="8"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="8"/>
+      <c r="D26" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>44</v>
-      </c>
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="6"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="8"/>
+      <c r="D27" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="6"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="8"/>
+      <c r="D28" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="6"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="16"/>
+      <c r="D29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
       <c r="C30" s="6"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="8"/>
+      <c r="D30" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
       <c r="C31" s="6"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="8"/>
+      <c r="D31" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
@@ -1373,9 +1405,7 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
-        <v>46</v>
-      </c>
+      <c r="A34" s="12"/>
       <c r="B34" s="13"/>
       <c r="C34" s="14"/>
       <c r="D34" s="7"/>
@@ -1383,60 +1413,40 @@
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>48</v>
-      </c>
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="6"/>
       <c r="D35" s="7"/>
       <c r="E35" s="5"/>
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
       <c r="C36" s="6"/>
       <c r="D36" s="7"/>
       <c r="E36" s="5"/>
       <c r="F36" s="8"/>
     </row>
     <row r="37" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
       <c r="C37" s="6"/>
       <c r="D37" s="15"/>
       <c r="E37" s="13"/>
       <c r="F37" s="16"/>
     </row>
     <row r="38" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
       <c r="C38" s="6"/>
       <c r="D38" s="7"/>
       <c r="E38" s="5"/>
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>56</v>
-      </c>
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
       <c r="C39" s="6"/>
       <c r="D39" s="7"/>
       <c r="E39" s="5"/>
@@ -1501,7 +1511,7 @@
       <c r="F45" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="D37:F37"/>
     <mergeCell ref="D40:F40"/>
@@ -1510,7 +1520,8 @@
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D26:F26"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Site updated: 2023-02-01 23:03:29
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B138CA69-12E1-481D-A508-DCA02F4D9F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD1B8B3-0558-448B-A7E5-FB074013100D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
   <si>
     <t>数组</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -273,6 +273,24 @@
   <si>
     <t>两个数组的交集</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>leetcode</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>leetcode 202</t>
+  </si>
+  <si>
+    <t>leetcode 202</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>快乐数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023-de-01</t>
   </si>
 </sst>
 </file>
@@ -947,7 +965,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1217,7 +1235,9 @@
       <c r="B17" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="6"/>
+      <c r="C17" s="6">
+        <v>44956</v>
+      </c>
       <c r="D17" s="4" t="s">
         <v>30</v>
       </c>
@@ -1233,7 +1253,9 @@
       <c r="B18" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="6">
+        <v>44957</v>
+      </c>
       <c r="D18" s="4" t="s">
         <v>34</v>
       </c>
@@ -1243,9 +1265,15 @@
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
+      <c r="A19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="6">
+        <v>44958</v>
+      </c>
       <c r="D19" s="4" t="s">
         <v>43</v>
       </c>
@@ -1255,9 +1283,13 @@
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
+      <c r="C20" s="6">
+        <v>44958</v>
+      </c>
       <c r="D20" s="4" t="s">
         <v>45</v>
       </c>
@@ -1267,9 +1299,13 @@
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+      <c r="A21" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
+      <c r="C21" s="6">
+        <v>44958</v>
+      </c>
       <c r="D21" s="4" t="s">
         <v>23</v>
       </c>
@@ -1279,9 +1315,13 @@
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
+      <c r="C22" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="D22" s="4" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Site updated: 2023-02-02 11:15:23
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD1B8B3-0558-448B-A7E5-FB074013100D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E109DE14-0CF6-47B4-BF4B-A4069B2B8AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
   <si>
     <t>数组</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -275,22 +275,12 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>leetcode</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>leetcode 202</t>
-  </si>
-  <si>
-    <t>leetcode 202</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>快乐数</t>
     <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023-de-01</t>
   </si>
 </sst>
 </file>
@@ -340,7 +330,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,6 +358,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -608,7 +604,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -677,6 +673,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -962,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1084,9 +1089,7 @@
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="22"/>
-      <c r="D8" s="20" t="s">
-        <v>29</v>
-      </c>
+      <c r="D8" s="20"/>
       <c r="E8" s="21"/>
       <c r="F8" s="22"/>
     </row>
@@ -1100,12 +1103,8 @@
       <c r="C9" s="6">
         <v>44949</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
@@ -1118,12 +1117,8 @@
       <c r="C10" s="6">
         <v>44950</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
@@ -1136,12 +1131,8 @@
       <c r="C11" s="6">
         <v>44951</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
@@ -1154,12 +1145,8 @@
       <c r="C12" s="6">
         <v>44952</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
@@ -1172,12 +1159,8 @@
       <c r="C13" s="6">
         <v>44953</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
@@ -1190,12 +1173,8 @@
       <c r="C14" s="6">
         <v>44954</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
@@ -1215,11 +1194,11 @@
       <c r="F15" s="23"/>
     </row>
     <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="4" t="s">
         <v>6</v>
       </c>
@@ -1266,10 +1245,10 @@
     </row>
     <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19" s="6">
         <v>44958</v>
@@ -1283,13 +1262,11 @@
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6">
-        <v>44958</v>
-      </c>
+      <c r="A20" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="4" t="s">
         <v>45</v>
       </c>
@@ -1300,11 +1277,13 @@
     </row>
     <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="C21" s="6">
-        <v>44958</v>
+        <v>44959</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>23</v>
@@ -1316,11 +1295,13 @@
     </row>
     <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6" t="s">
-        <v>66</v>
+        <v>32</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="6">
+        <v>44959</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>25</v>
@@ -1331,9 +1312,15 @@
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="23"/>
+      <c r="A23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="6">
+        <v>44959</v>
+      </c>
       <c r="D23" s="4" t="s">
         <v>27</v>
       </c>
@@ -1343,52 +1330,72 @@
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
+      <c r="A24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="6">
+        <v>44959</v>
+      </c>
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
+      <c r="A25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="6">
+        <v>44959</v>
+      </c>
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
       <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="12" t="s">
+      <c r="A26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="6">
+        <v>44959</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="6">
+        <v>44959</v>
+      </c>
+      <c r="D27" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="14"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" s="6"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
       <c r="D28" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F28" s="6"/>
     </row>
@@ -1397,10 +1404,10 @@
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
       <c r="D29" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F29" s="6"/>
     </row>
@@ -1409,10 +1416,10 @@
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
       <c r="D30" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F30" s="6"/>
     </row>
@@ -1421,10 +1428,10 @@
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
       <c r="D31" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F31" s="6"/>
     </row>
@@ -1432,9 +1439,13 @@
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="8"/>
+      <c r="D32" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
@@ -1445,17 +1456,17 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="14"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
       <c r="D34" s="7"/>
       <c r="E34" s="5"/>
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="6"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="14"/>
       <c r="D35" s="7"/>
       <c r="E35" s="5"/>
       <c r="F35" s="8"/>
@@ -1472,17 +1483,17 @@
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="6"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="16"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="8"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="16"/>
     </row>
     <row r="39" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
@@ -1496,33 +1507,29 @@
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="6"/>
-      <c r="D40" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="14"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
-      <c r="D41" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F41" s="6"/>
+      <c r="D41" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="13"/>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="C42" s="6"/>
       <c r="D42" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F42" s="6"/>
     </row>
@@ -1530,9 +1537,13 @@
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="C43" s="6"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="8"/>
+      <c r="D43" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F43" s="6"/>
     </row>
     <row r="44" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
@@ -1550,18 +1561,26 @@
       <c r="E45" s="5"/>
       <c r="F45" s="8"/>
     </row>
+    <row r="46" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="8"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D41:F41"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A23:C23"/>
     <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="A20:C20"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Site updated: 2023-02-03 18:28:52
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E109DE14-0CF6-47B4-BF4B-A4069B2B8AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476B3BFD-5D89-46C0-838D-7DEEF7B02511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -672,16 +672,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -970,7 +970,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1191,14 +1191,14 @@
         <v>42</v>
       </c>
       <c r="E15" s="21"/>
-      <c r="F15" s="23"/>
+      <c r="F15" s="26"/>
     </row>
     <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="4" t="s">
         <v>6</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>33</v>
       </c>
       <c r="C22" s="6">
-        <v>44959</v>
+        <v>44960</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Site updated: 2023-02-04 14:08:44
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476B3BFD-5D89-46C0-838D-7DEEF7B02511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F02FBE-CB5B-41E0-9542-214575E55479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1319,7 +1319,7 @@
         <v>35</v>
       </c>
       <c r="C23" s="6">
-        <v>44959</v>
+        <v>44961</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Site updated: 2023-02-05 14:12:02
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F02FBE-CB5B-41E0-9542-214575E55479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC1CD15-7199-4748-A5F0-07EDF4C803E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -970,7 +970,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1337,7 +1337,7 @@
         <v>44</v>
       </c>
       <c r="C24" s="6">
-        <v>44959</v>
+        <v>44962</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>

</xml_diff>

<commit_message>
Site updated: 2023-02-06 15:12:11
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC1CD15-7199-4748-A5F0-07EDF4C803E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55827C1B-5137-4053-B4FA-A7B038B851FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -970,7 +970,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1351,7 +1351,7 @@
         <v>37</v>
       </c>
       <c r="C25" s="6">
-        <v>44959</v>
+        <v>44963</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>

</xml_diff>

<commit_message>
Site updated: 2023-03-07 12:03:27
</commit_message>
<xml_diff>
--- a/leetcode/刷题日志.xlsx
+++ b/leetcode/刷题日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\Blog\source\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55827C1B-5137-4053-B4FA-A7B038B851FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF441125-ABFA-4091-A6BD-70695889EEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,10 +183,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>实现 strStr()</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>leetcode 459</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -280,6 +276,10 @@
   </si>
   <si>
     <t>快乐数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>找出字符串中第一个匹配项的下标</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -604,7 +604,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -682,6 +682,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="6" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -969,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1188,14 +1197,14 @@
         <v>44955</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="21"/>
       <c r="F15" s="26"/>
     </row>
     <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="24"/>
       <c r="C16" s="25"/>
@@ -1209,10 +1218,10 @@
     </row>
     <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="C17" s="6">
         <v>44956</v>
@@ -1227,10 +1236,10 @@
     </row>
     <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="C18" s="6">
         <v>44957</v>
@@ -1245,19 +1254,19 @@
     </row>
     <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="C19" s="6">
         <v>44958</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="F19" s="6"/>
     </row>
@@ -1268,7 +1277,7 @@
       <c r="B20" s="21"/>
       <c r="C20" s="22"/>
       <c r="D20" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>20</v>
@@ -1331,10 +1340,10 @@
     </row>
     <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="C24" s="6">
         <v>44962</v>
@@ -1358,14 +1367,14 @@
       <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="6">
-        <v>44959</v>
+      <c r="B26" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="29">
+        <v>44964</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
@@ -1373,16 +1382,16 @@
     </row>
     <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="C27" s="6">
-        <v>44959</v>
+        <v>44965</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
@@ -1392,10 +1401,10 @@
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
       <c r="D28" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="F28" s="6"/>
     </row>
@@ -1404,10 +1413,10 @@
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
       <c r="D29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="F29" s="6"/>
     </row>
@@ -1416,10 +1425,10 @@
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
       <c r="D30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="F30" s="6"/>
     </row>
@@ -1428,10 +1437,10 @@
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
       <c r="D31" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="F31" s="6"/>
     </row>
@@ -1440,10 +1449,10 @@
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
       <c r="D32" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="F32" s="6"/>
     </row>
@@ -1516,7 +1525,7 @@
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
       <c r="D41" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E41" s="13"/>
       <c r="F41" s="14"/>
@@ -1526,10 +1535,10 @@
       <c r="B42" s="5"/>
       <c r="C42" s="6"/>
       <c r="D42" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="F42" s="6"/>
     </row>
@@ -1538,10 +1547,10 @@
       <c r="B43" s="5"/>
       <c r="C43" s="6"/>
       <c r="D43" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="F43" s="6"/>
     </row>

</xml_diff>